<commit_message>
fix(req3): :bug: fix wrong data in database inputs
</commit_message>
<xml_diff>
--- a/SpotifyClone-Tables.xlsx
+++ b/SpotifyClone-Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\julianoboese\documents\trybe\trybe-entrega-projetos\back-end\bloco-21-funcoes-sql-joins-e-normalizacao\mysql-one-for-all\sd-018-b-mysql-one-for-all\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E21854E-F197-490C-ADF7-67D82B98CC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3605085-6A39-4D0C-A44E-65798F152AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="28800" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15712,8 +15712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6949EDD-2D55-4284-8681-43AA46BDFCDE}">
   <dimension ref="A1:S999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15963,7 +15963,7 @@
         <v>128</v>
       </c>
       <c r="L5" s="37">
-        <v>190</v>
+        <v>241</v>
       </c>
       <c r="M5" s="37">
         <v>6</v>
@@ -16690,7 +16690,7 @@
         <v>144</v>
       </c>
       <c r="L21" s="37">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="M21" s="37">
         <v>8</v>
@@ -17425,7 +17425,7 @@
         <v>163</v>
       </c>
       <c r="L40" s="35">
-        <v>203</v>
+        <v>83</v>
       </c>
       <c r="M40" s="35">
         <v>2</v>
@@ -17449,7 +17449,7 @@
         <v>164</v>
       </c>
       <c r="L41" s="37">
-        <v>240</v>
+        <v>197</v>
       </c>
       <c r="M41" s="37">
         <v>5</v>

</xml_diff>